<commit_message>
fix: retrained model to better map dataset labels to numerical values
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -968,12 +968,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="2">
-    <tableStyle name="Form Responses 1-style" pivot="0" count="3" xr9:uid="{1A8017D8-6108-4188-B1B1-27C3D0DC6708}">
+    <tableStyle name="Form Responses 1-style" pivot="0" count="3" xr9:uid="{BD35C5C3-F0A3-4ED5-91A3-BEC8EFC57A8B}">
       <tableStyleElement type="headerRow" dxfId="13"/>
       <tableStyleElement type="firstRowStripe" dxfId="12"/>
       <tableStyleElement type="secondRowStripe" dxfId="11"/>
     </tableStyle>
-    <tableStyle name="Sheet1-style" pivot="0" count="2" xr9:uid="{7CD90335-871A-4D04-9D83-C41E95E55DE5}">
+    <tableStyle name="Sheet1-style" pivot="0" count="2" xr9:uid="{6149C924-75F6-4582-BA9D-468BE72B27FB}">
       <tableStyleElement type="firstRowStripe" dxfId="15"/>
       <tableStyleElement type="secondRowStripe" dxfId="14"/>
     </tableStyle>
@@ -1208,7 +1208,7 @@
   <dimension ref="A1:Y971"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
feat: added job title prediction
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="48">
   <si>
     <t>PracticumGrade</t>
   </si>
@@ -62,6 +62,9 @@
     <t>TimeToEmployment</t>
   </si>
   <si>
+    <t>JobTitle</t>
+  </si>
+  <si>
     <t>Above Average (1.0 - 1.5)</t>
   </si>
   <si>
@@ -71,10 +74,22 @@
     <t>Yes</t>
   </si>
   <si>
+    <t>API developer</t>
+  </si>
+  <si>
     <t>Average (1.75 - 2.5)</t>
   </si>
   <si>
+    <t>fullstack developer</t>
+  </si>
+  <si>
+    <t>Associate Software Engineer</t>
+  </si>
+  <si>
     <t>High</t>
+  </si>
+  <si>
+    <t>Cadet Engineer</t>
   </si>
   <si>
     <t>Below Average (2.75 - 5)</t>
@@ -83,7 +98,79 @@
     <t>No</t>
   </si>
   <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
     <t>Moderate</t>
+  </si>
+  <si>
+    <t>Staff Consultant</t>
+  </si>
+  <si>
+    <t>Software Developer</t>
+  </si>
+  <si>
+    <t>Fullstack developer</t>
+  </si>
+  <si>
+    <t>software developer</t>
+  </si>
+  <si>
+    <t>Programmer Analyst</t>
+  </si>
+  <si>
+    <t>software engineer - graduate program</t>
+  </si>
+  <si>
+    <t>Analyst</t>
+  </si>
+  <si>
+    <t>Platform Engineer</t>
+  </si>
+  <si>
+    <t>Junior Software Engineer</t>
+  </si>
+  <si>
+    <t>Cloud Operations Apprentice</t>
+  </si>
+  <si>
+    <t>Junior Backend Web Developer</t>
+  </si>
+  <si>
+    <t>Associate Data Scientist</t>
+  </si>
+  <si>
+    <t>Software Engineer (Graduate Program)</t>
+  </si>
+  <si>
+    <t>Game Developer</t>
+  </si>
+  <si>
+    <t>Junior Backend Developer</t>
+  </si>
+  <si>
+    <t>Junior Desktop Technician</t>
+  </si>
+  <si>
+    <t>Junior Associate Software Developer</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>Technical Consultant</t>
+  </si>
+  <si>
+    <t>Fullstack Developer</t>
+  </si>
+  <si>
+    <t>Software engineer</t>
+  </si>
+  <si>
+    <t>Cloud Solutions Architect</t>
+  </si>
+  <si>
+    <t>Product Owner Associate</t>
   </si>
 </sst>
 </file>
@@ -263,12 +350,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F9FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -457,12 +556,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -587,7 +701,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -599,125 +713,134 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -968,12 +1091,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="2">
-    <tableStyle name="Form Responses 1-style" pivot="0" count="3" xr9:uid="{BD35C5C3-F0A3-4ED5-91A3-BEC8EFC57A8B}">
+    <tableStyle name="Form Responses 1-style" pivot="0" count="3" xr9:uid="{F33606FC-25CE-4470-BFB1-C58FC53509A1}">
       <tableStyleElement type="headerRow" dxfId="13"/>
       <tableStyleElement type="firstRowStripe" dxfId="12"/>
       <tableStyleElement type="secondRowStripe" dxfId="11"/>
     </tableStyle>
-    <tableStyle name="Sheet1-style" pivot="0" count="2" xr9:uid="{6149C924-75F6-4582-BA9D-468BE72B27FB}">
+    <tableStyle name="Sheet1-style" pivot="0" count="2" xr9:uid="{5D4B1883-A6E0-42A6-BB38-72CB57C52B4E}">
       <tableStyleElement type="firstRowStripe" dxfId="15"/>
       <tableStyleElement type="secondRowStripe" dxfId="14"/>
     </tableStyle>
@@ -987,7 +1110,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_1" displayName="Table_1" ref="A2:K50" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_1" displayName="Table_1" ref="A2:K43" headerRowCount="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column1" dataDxfId="0"/>
     <tableColumn id="2" name="Column2" dataDxfId="1"/>
@@ -1205,10 +1328,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y971"/>
+  <dimension ref="A1:Y964"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1"/>
@@ -1247,7 +1370,9 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1"/>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -1264,39 +1389,41 @@
     </row>
     <row r="2" customHeight="1" spans="1:25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K2" s="2">
         <v>2</v>
       </c>
-      <c r="L2" s="1"/>
+      <c r="L2" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -1313,39 +1440,41 @@
     </row>
     <row r="3" customHeight="1" spans="1:25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="K3" s="2">
         <v>0</v>
       </c>
-      <c r="L3" s="1"/>
+      <c r="L3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -1362,39 +1491,41 @@
     </row>
     <row r="4" customHeight="1" spans="1:25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="K4" s="2">
         <v>3</v>
       </c>
-      <c r="L4" s="1"/>
+      <c r="L4" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -1411,39 +1542,41 @@
     </row>
     <row r="5" customHeight="1" spans="1:25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K5" s="2">
         <v>1</v>
       </c>
-      <c r="L5" s="1"/>
+      <c r="L5" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1460,39 +1593,41 @@
     </row>
     <row r="6" customHeight="1" spans="1:25">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K6" s="2">
         <v>2</v>
       </c>
-      <c r="L6" s="1"/>
+      <c r="L6" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -1509,39 +1644,41 @@
     </row>
     <row r="7" customHeight="1" spans="1:25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K7" s="2">
         <v>0.3</v>
       </c>
-      <c r="L7" s="1"/>
+      <c r="L7" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1558,39 +1695,41 @@
     </row>
     <row r="8" customHeight="1" spans="1:25">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K8" s="2">
         <v>1</v>
       </c>
-      <c r="L8" s="1"/>
+      <c r="L8" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -1607,39 +1746,41 @@
     </row>
     <row r="9" customHeight="1" spans="1:25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="K9" s="2">
         <v>2</v>
       </c>
-      <c r="L9" s="1"/>
+      <c r="L9" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -1656,39 +1797,41 @@
     </row>
     <row r="10" customHeight="1" spans="1:25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="K10" s="2">
         <v>3</v>
       </c>
-      <c r="L10" s="1"/>
+      <c r="L10" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -1705,39 +1848,41 @@
     </row>
     <row r="11" customHeight="1" spans="1:25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K11" s="2">
         <v>0</v>
       </c>
-      <c r="L11" s="1"/>
+      <c r="L11" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1754,39 +1899,41 @@
     </row>
     <row r="12" customHeight="1" spans="1:25">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K12" s="2">
         <v>2</v>
       </c>
-      <c r="L12" s="1"/>
+      <c r="L12" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1803,39 +1950,41 @@
     </row>
     <row r="13" customHeight="1" spans="1:25">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="K13" s="2">
         <v>2</v>
       </c>
-      <c r="L13" s="1"/>
+      <c r="L13" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1852,39 +2001,41 @@
     </row>
     <row r="14" customHeight="1" spans="1:25">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K14" s="2">
         <v>2</v>
       </c>
-      <c r="L14" s="1"/>
+      <c r="L14" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -1901,39 +2052,41 @@
     </row>
     <row r="15" customHeight="1" spans="1:25">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K15" s="2">
         <v>1</v>
       </c>
-      <c r="L15" s="1"/>
+      <c r="L15" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1950,39 +2103,41 @@
     </row>
     <row r="16" customHeight="1" spans="1:25">
       <c r="A16" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K16" s="2">
         <v>2</v>
       </c>
-      <c r="L16" s="1"/>
+      <c r="L16" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1999,39 +2154,41 @@
     </row>
     <row r="17" customHeight="1" spans="1:25">
       <c r="A17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="K17" s="2">
         <v>2</v>
       </c>
-      <c r="L17" s="1"/>
+      <c r="L17" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -2048,39 +2205,41 @@
     </row>
     <row r="18" customHeight="1" spans="1:25">
       <c r="A18" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K18" s="2">
         <v>1</v>
       </c>
-      <c r="L18" s="1"/>
+      <c r="L18" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -2097,39 +2256,41 @@
     </row>
     <row r="19" customHeight="1" spans="1:25">
       <c r="A19" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="K19" s="2">
         <v>1</v>
       </c>
-      <c r="L19" s="1"/>
+      <c r="L19" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -2146,39 +2307,41 @@
     </row>
     <row r="20" customHeight="1" spans="1:25">
       <c r="A20" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="K20" s="2">
         <v>1</v>
       </c>
-      <c r="L20" s="1"/>
+      <c r="L20" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -2195,39 +2358,41 @@
     </row>
     <row r="21" customHeight="1" spans="1:25">
       <c r="A21" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="K21" s="2">
         <v>1</v>
       </c>
-      <c r="L21" s="1"/>
+      <c r="L21" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -2244,39 +2409,41 @@
     </row>
     <row r="22" customHeight="1" spans="1:25">
       <c r="A22" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K22" s="2">
         <v>2</v>
       </c>
-      <c r="L22" s="1"/>
+      <c r="L22" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -2293,39 +2460,41 @@
     </row>
     <row r="23" customHeight="1" spans="1:25">
       <c r="A23" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K23" s="2">
         <v>2</v>
       </c>
-      <c r="L23" s="1"/>
+      <c r="L23" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -2341,18 +2510,42 @@
       <c r="Y23" s="1"/>
     </row>
     <row r="24" customHeight="1" spans="1:25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K24" s="2">
+        <v>2</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
@@ -2369,39 +2562,41 @@
     </row>
     <row r="25" customHeight="1" spans="1:25">
       <c r="A25" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="K25" s="2">
-        <v>2</v>
-      </c>
-      <c r="L25" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -2418,39 +2613,41 @@
     </row>
     <row r="26" customHeight="1" spans="1:25">
       <c r="A26" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J26" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="K26" s="2">
         <v>1</v>
       </c>
-      <c r="L26" s="1"/>
+      <c r="L26" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -2466,18 +2663,42 @@
       <c r="Y26" s="1"/>
     </row>
     <row r="27" customHeight="1" spans="1:25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" s="2">
+        <v>4</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
@@ -2494,39 +2715,41 @@
     </row>
     <row r="28" customHeight="1" spans="1:25">
       <c r="A28" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="K28" s="2">
-        <v>1</v>
-      </c>
-      <c r="L28" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
@@ -2543,39 +2766,41 @@
     </row>
     <row r="29" customHeight="1" spans="1:25">
       <c r="A29" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="K29" s="2">
-        <v>4</v>
-      </c>
-      <c r="L29" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
@@ -2592,39 +2817,41 @@
     </row>
     <row r="30" customHeight="1" spans="1:25">
       <c r="A30" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K30" s="2">
-        <v>2</v>
-      </c>
-      <c r="L30" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
@@ -2641,39 +2868,41 @@
     </row>
     <row r="31" customHeight="1" spans="1:25">
       <c r="A31" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J31" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="K31" s="2">
-        <v>3</v>
-      </c>
-      <c r="L31" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -2690,39 +2919,41 @@
     </row>
     <row r="32" customHeight="1" spans="1:25">
       <c r="A32" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="K32" s="2">
         <v>1</v>
       </c>
-      <c r="L32" s="1"/>
+      <c r="L32" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -2739,39 +2970,41 @@
     </row>
     <row r="33" customHeight="1" spans="1:25">
       <c r="A33" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="K33" s="2">
-        <v>2</v>
-      </c>
-      <c r="L33" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
@@ -2788,39 +3021,41 @@
     </row>
     <row r="34" customHeight="1" spans="1:25">
       <c r="A34" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K34" s="2">
-        <v>1</v>
-      </c>
-      <c r="L34" s="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -2837,7 +3072,7 @@
     </row>
     <row r="35" customHeight="1" spans="1:25">
       <c r="A35" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>16</v>
@@ -2846,30 +3081,32 @@
         <v>16</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K35" s="2">
-        <v>1</v>
-      </c>
-      <c r="L35" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
@@ -2886,39 +3123,41 @@
     </row>
     <row r="36" customHeight="1" spans="1:25">
       <c r="A36" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="K36" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="L36" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
@@ -2935,39 +3174,41 @@
     </row>
     <row r="37" customHeight="1" spans="1:25">
       <c r="A37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J37" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="K37" s="2">
-        <v>3</v>
-      </c>
-      <c r="L37" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
@@ -2984,39 +3225,41 @@
     </row>
     <row r="38" customHeight="1" spans="1:25">
       <c r="A38" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K38" s="2">
-        <v>0</v>
-      </c>
-      <c r="L38" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
@@ -3033,39 +3276,41 @@
     </row>
     <row r="39" customHeight="1" spans="1:25">
       <c r="A39" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="K39" s="2">
-        <v>4</v>
-      </c>
-      <c r="L39" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="L39" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
@@ -3082,39 +3327,41 @@
     </row>
     <row r="40" customHeight="1" spans="1:25">
       <c r="A40" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K40" s="2">
-        <v>1</v>
-      </c>
-      <c r="L40" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
@@ -3131,39 +3378,41 @@
     </row>
     <row r="41" customHeight="1" spans="1:25">
       <c r="A41" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K41" s="2">
-        <v>10</v>
-      </c>
-      <c r="L41" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="L41" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
@@ -3179,18 +3428,42 @@
       <c r="Y41" s="1"/>
     </row>
     <row r="42" customHeight="1" spans="1:25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="1"/>
+      <c r="A42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K42" s="2">
+        <v>2</v>
+      </c>
+      <c r="L42" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
@@ -3207,39 +3480,41 @@
     </row>
     <row r="43" customHeight="1" spans="1:25">
       <c r="A43" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K43" s="2">
-        <v>3</v>
-      </c>
-      <c r="L43" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="L43" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
@@ -3255,39 +3530,17 @@
       <c r="Y43" s="1"/>
     </row>
     <row r="44" customHeight="1" spans="1:25">
-      <c r="A44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K44" s="2">
-        <v>0</v>
-      </c>
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
@@ -3306,15 +3559,15 @@
     <row r="45" customHeight="1" spans="1:25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
@@ -3331,39 +3584,17 @@
       <c r="Y45" s="1"/>
     </row>
     <row r="46" customHeight="1" spans="1:25">
-      <c r="A46" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K46" s="2">
-        <v>2</v>
-      </c>
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
@@ -3382,15 +3613,15 @@
     <row r="47" customHeight="1" spans="1:25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
@@ -3407,39 +3638,17 @@
       <c r="Y47" s="1"/>
     </row>
     <row r="48" customHeight="1" spans="1:25">
-      <c r="A48" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K48" s="2">
-        <v>2</v>
-      </c>
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
@@ -3458,15 +3667,15 @@
     <row r="49" customHeight="1" spans="1:25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
@@ -3485,15 +3694,15 @@
     <row r="50" customHeight="1" spans="1:25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
@@ -28187,195 +28396,6 @@
       <c r="X964" s="1"/>
       <c r="Y964" s="1"/>
     </row>
-    <row r="965" customHeight="1" spans="1:25">
-      <c r="A965" s="1"/>
-      <c r="B965" s="1"/>
-      <c r="C965" s="1"/>
-      <c r="D965" s="1"/>
-      <c r="E965" s="1"/>
-      <c r="F965" s="1"/>
-      <c r="G965" s="1"/>
-      <c r="H965" s="1"/>
-      <c r="I965" s="1"/>
-      <c r="J965" s="1"/>
-      <c r="K965" s="1"/>
-      <c r="L965" s="1"/>
-      <c r="M965" s="1"/>
-      <c r="N965" s="1"/>
-      <c r="O965" s="1"/>
-      <c r="P965" s="1"/>
-      <c r="Q965" s="1"/>
-      <c r="R965" s="1"/>
-      <c r="S965" s="1"/>
-      <c r="T965" s="1"/>
-      <c r="U965" s="1"/>
-      <c r="V965" s="1"/>
-      <c r="W965" s="1"/>
-      <c r="X965" s="1"/>
-      <c r="Y965" s="1"/>
-    </row>
-    <row r="966" customHeight="1" spans="1:25">
-      <c r="A966" s="1"/>
-      <c r="B966" s="1"/>
-      <c r="C966" s="1"/>
-      <c r="D966" s="1"/>
-      <c r="E966" s="1"/>
-      <c r="F966" s="1"/>
-      <c r="G966" s="1"/>
-      <c r="H966" s="1"/>
-      <c r="I966" s="1"/>
-      <c r="J966" s="1"/>
-      <c r="K966" s="1"/>
-      <c r="L966" s="1"/>
-      <c r="M966" s="1"/>
-      <c r="N966" s="1"/>
-      <c r="O966" s="1"/>
-      <c r="P966" s="1"/>
-      <c r="Q966" s="1"/>
-      <c r="R966" s="1"/>
-      <c r="S966" s="1"/>
-      <c r="T966" s="1"/>
-      <c r="U966" s="1"/>
-      <c r="V966" s="1"/>
-      <c r="W966" s="1"/>
-      <c r="X966" s="1"/>
-      <c r="Y966" s="1"/>
-    </row>
-    <row r="967" customHeight="1" spans="1:25">
-      <c r="A967" s="1"/>
-      <c r="B967" s="1"/>
-      <c r="C967" s="1"/>
-      <c r="D967" s="1"/>
-      <c r="E967" s="1"/>
-      <c r="F967" s="1"/>
-      <c r="G967" s="1"/>
-      <c r="H967" s="1"/>
-      <c r="I967" s="1"/>
-      <c r="J967" s="1"/>
-      <c r="K967" s="1"/>
-      <c r="L967" s="1"/>
-      <c r="M967" s="1"/>
-      <c r="N967" s="1"/>
-      <c r="O967" s="1"/>
-      <c r="P967" s="1"/>
-      <c r="Q967" s="1"/>
-      <c r="R967" s="1"/>
-      <c r="S967" s="1"/>
-      <c r="T967" s="1"/>
-      <c r="U967" s="1"/>
-      <c r="V967" s="1"/>
-      <c r="W967" s="1"/>
-      <c r="X967" s="1"/>
-      <c r="Y967" s="1"/>
-    </row>
-    <row r="968" customHeight="1" spans="1:25">
-      <c r="A968" s="1"/>
-      <c r="B968" s="1"/>
-      <c r="C968" s="1"/>
-      <c r="D968" s="1"/>
-      <c r="E968" s="1"/>
-      <c r="F968" s="1"/>
-      <c r="G968" s="1"/>
-      <c r="H968" s="1"/>
-      <c r="I968" s="1"/>
-      <c r="J968" s="1"/>
-      <c r="K968" s="1"/>
-      <c r="L968" s="1"/>
-      <c r="M968" s="1"/>
-      <c r="N968" s="1"/>
-      <c r="O968" s="1"/>
-      <c r="P968" s="1"/>
-      <c r="Q968" s="1"/>
-      <c r="R968" s="1"/>
-      <c r="S968" s="1"/>
-      <c r="T968" s="1"/>
-      <c r="U968" s="1"/>
-      <c r="V968" s="1"/>
-      <c r="W968" s="1"/>
-      <c r="X968" s="1"/>
-      <c r="Y968" s="1"/>
-    </row>
-    <row r="969" customHeight="1" spans="1:25">
-      <c r="A969" s="1"/>
-      <c r="B969" s="1"/>
-      <c r="C969" s="1"/>
-      <c r="D969" s="1"/>
-      <c r="E969" s="1"/>
-      <c r="F969" s="1"/>
-      <c r="G969" s="1"/>
-      <c r="H969" s="1"/>
-      <c r="I969" s="1"/>
-      <c r="J969" s="1"/>
-      <c r="K969" s="1"/>
-      <c r="L969" s="1"/>
-      <c r="M969" s="1"/>
-      <c r="N969" s="1"/>
-      <c r="O969" s="1"/>
-      <c r="P969" s="1"/>
-      <c r="Q969" s="1"/>
-      <c r="R969" s="1"/>
-      <c r="S969" s="1"/>
-      <c r="T969" s="1"/>
-      <c r="U969" s="1"/>
-      <c r="V969" s="1"/>
-      <c r="W969" s="1"/>
-      <c r="X969" s="1"/>
-      <c r="Y969" s="1"/>
-    </row>
-    <row r="970" customHeight="1" spans="1:25">
-      <c r="A970" s="1"/>
-      <c r="B970" s="1"/>
-      <c r="C970" s="1"/>
-      <c r="D970" s="1"/>
-      <c r="E970" s="1"/>
-      <c r="F970" s="1"/>
-      <c r="G970" s="1"/>
-      <c r="H970" s="1"/>
-      <c r="I970" s="1"/>
-      <c r="J970" s="1"/>
-      <c r="K970" s="1"/>
-      <c r="L970" s="1"/>
-      <c r="M970" s="1"/>
-      <c r="N970" s="1"/>
-      <c r="O970" s="1"/>
-      <c r="P970" s="1"/>
-      <c r="Q970" s="1"/>
-      <c r="R970" s="1"/>
-      <c r="S970" s="1"/>
-      <c r="T970" s="1"/>
-      <c r="U970" s="1"/>
-      <c r="V970" s="1"/>
-      <c r="W970" s="1"/>
-      <c r="X970" s="1"/>
-      <c r="Y970" s="1"/>
-    </row>
-    <row r="971" customHeight="1" spans="1:25">
-      <c r="A971" s="1"/>
-      <c r="B971" s="1"/>
-      <c r="C971" s="1"/>
-      <c r="D971" s="1"/>
-      <c r="E971" s="1"/>
-      <c r="F971" s="1"/>
-      <c r="G971" s="1"/>
-      <c r="H971" s="1"/>
-      <c r="I971" s="1"/>
-      <c r="J971" s="1"/>
-      <c r="K971" s="1"/>
-      <c r="L971" s="1"/>
-      <c r="M971" s="1"/>
-      <c r="N971" s="1"/>
-      <c r="O971" s="1"/>
-      <c r="P971" s="1"/>
-      <c r="Q971" s="1"/>
-      <c r="R971" s="1"/>
-      <c r="S971" s="1"/>
-      <c r="T971" s="1"/>
-      <c r="U971" s="1"/>
-      <c r="V971" s="1"/>
-      <c r="W971" s="1"/>
-      <c r="X971" s="1"/>
-      <c r="Y971" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>